<commit_message>
Fix code review feedback: remove unused imports, fix unused variables, add Assigned_Agent validation, fix formula to return 0, use date objects, apply base setup to all tabs, fix linting issues
Co-authored-by: natbkgift <40134401+natbkgift@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/data/templates/Property_Master_List.xlsx
+++ b/docs/data/templates/Property_Master_List.xlsx
@@ -23,7 +23,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <name val="Calibri"/>
@@ -95,18 +98,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -908,7 +912,7 @@
         </is>
       </c>
       <c r="O2">
-        <f>IF(AND(L2&gt;0, V2&gt;0), L2/V2, "N/A")</f>
+        <f>IF(AND(L2&gt;0, V2&gt;0), L2/V2, 0)</f>
         <v/>
       </c>
       <c r="P2" t="inlineStr">
@@ -1000,15 +1004,11 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="AS2" t="inlineStr">
-        <is>
-          <t>2026-01-26</t>
-        </is>
-      </c>
-      <c r="AT2" t="inlineStr">
-        <is>
-          <t>2026-01-26</t>
-        </is>
+      <c r="AS2" s="2" t="n">
+        <v>46048</v>
+      </c>
+      <c r="AT2" s="2" t="n">
+        <v>46048</v>
       </c>
       <c r="AV2" t="n">
         <v>15</v>
@@ -1056,7 +1056,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="17">
+  <dataValidations count="18">
     <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
       <formula1>"Available,Reserved,Sold,Rented,Pending,Off Market"</formula1>
     </dataValidation>
@@ -1089,6 +1089,9 @@
     </dataValidation>
     <dataValidation sqref="AM2:AM1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
       <formula1>"Owner Direct,Agent,LINE Group,Facebook,Website,Walk-in,Referral"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AO2:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Somchai S.,Napat K.,John D.,Sarah M.,Unassigned"</formula1>
     </dataValidation>
     <dataValidation sqref="AP2:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
       <formula1>"Low,Medium,High"</formula1>
@@ -1129,340 +1132,459 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="15" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="30" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
+    <col width="12" customWidth="1" min="30" max="30"/>
+    <col width="12" customWidth="1" min="31" max="31"/>
+    <col width="15" customWidth="1" min="32" max="32"/>
+    <col width="20" customWidth="1" min="33" max="33"/>
+    <col width="15" customWidth="1" min="34" max="34"/>
+    <col width="15" customWidth="1" min="35" max="35"/>
+    <col width="15" customWidth="1" min="36" max="36"/>
+    <col width="15" customWidth="1" min="37" max="37"/>
+    <col width="15" customWidth="1" min="38" max="38"/>
+    <col width="15" customWidth="1" min="39" max="39"/>
+    <col width="25" customWidth="1" min="40" max="40"/>
+    <col width="15" customWidth="1" min="41" max="41"/>
+    <col width="12" customWidth="1" min="42" max="42"/>
+    <col width="12" customWidth="1" min="43" max="43"/>
+    <col width="12" customWidth="1" min="44" max="44"/>
+    <col width="12" customWidth="1" min="45" max="45"/>
+    <col width="12" customWidth="1" min="46" max="46"/>
+    <col width="12" customWidth="1" min="47" max="47"/>
+    <col width="12" customWidth="1" min="48" max="48"/>
+    <col width="12" customWidth="1" min="49" max="49"/>
+    <col width="30" customWidth="1" min="50" max="50"/>
+    <col width="20" customWidth="1" min="51" max="51"/>
+    <col width="12" customWidth="1" min="52" max="52"/>
+    <col width="40" customWidth="1" min="53" max="53"/>
+    <col width="40" customWidth="1" min="54" max="54"/>
+    <col width="12" customWidth="1" min="55" max="55"/>
+    <col width="10" customWidth="1" min="56" max="56"/>
+    <col width="12" customWidth="1" min="57" max="57"/>
+    <col width="15" customWidth="1" min="58" max="58"/>
+    <col width="12" customWidth="1" min="59" max="59"/>
+    <col width="15" customWidth="1" min="60" max="60"/>
+    <col width="15" customWidth="1" min="61" max="61"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Property_ID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Project_Name</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Unit_Number</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Location_Area</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Location_Sub</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Latitude</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Longitude</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Price_Sale</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Price_Rent</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="O1" s="2" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Price_Per_SQM</t>
         </is>
       </c>
-      <c r="P1" s="2" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Negotiable</t>
         </is>
       </c>
-      <c r="Q1" s="2" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Commission_Rate</t>
         </is>
       </c>
-      <c r="R1" s="2" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Owner_Type</t>
         </is>
       </c>
-      <c r="S1" s="2" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Foreign_Quota</t>
         </is>
       </c>
-      <c r="T1" s="2" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Bedrooms</t>
         </is>
       </c>
-      <c r="U1" s="2" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Bathrooms</t>
         </is>
       </c>
-      <c r="V1" s="2" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Size_SQM</t>
         </is>
       </c>
-      <c r="W1" s="2" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Size_SQW</t>
         </is>
       </c>
-      <c r="X1" s="2" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Floor_Level</t>
         </is>
       </c>
-      <c r="Y1" s="2" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>View</t>
         </is>
       </c>
-      <c r="Z1" s="2" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Furnishing</t>
         </is>
       </c>
-      <c r="AA1" s="2" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Parking</t>
         </is>
       </c>
-      <c r="AB1" s="2" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Facilities</t>
         </is>
       </c>
-      <c r="AC1" s="2" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Condition</t>
         </is>
       </c>
-      <c r="AD1" s="2" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Year_Built</t>
         </is>
       </c>
-      <c r="AE1" s="2" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Year_Renovated</t>
         </is>
       </c>
-      <c r="AF1" s="2" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Title_Deed</t>
         </is>
       </c>
-      <c r="AG1" s="2" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Developer</t>
         </is>
       </c>
-      <c r="AH1" s="2" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Photos_Link</t>
         </is>
       </c>
-      <c r="AI1" s="2" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Video_Link</t>
         </is>
       </c>
-      <c r="AJ1" s="2" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Brochure_Link</t>
         </is>
       </c>
-      <c r="AK1" s="2" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Virtual_Tour</t>
         </is>
       </c>
-      <c r="AL1" s="2" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Listing_URL</t>
         </is>
       </c>
-      <c r="AM1" s="2" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="AN1" s="2" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Source_Contact</t>
         </is>
       </c>
-      <c r="AO1" s="2" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Assigned_Agent</t>
         </is>
       </c>
-      <c r="AP1" s="2" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="AQ1" s="2" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Featured</t>
         </is>
       </c>
-      <c r="AR1" s="2" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Active_Marketing</t>
         </is>
       </c>
-      <c r="AS1" s="2" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Date_Added</t>
         </is>
       </c>
-      <c r="AT1" s="2" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Date_Updated</t>
         </is>
       </c>
-      <c r="AU1" s="2" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Date_Available</t>
         </is>
       </c>
-      <c r="AV1" s="2" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Views_Count</t>
         </is>
       </c>
-      <c r="AW1" s="2" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Viewings_Count</t>
         </is>
       </c>
-      <c r="AX1" s="2" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Notes_Internal</t>
         </is>
       </c>
-      <c r="AY1" s="2" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Tags</t>
         </is>
       </c>
-      <c r="AZ1" s="2" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Language</t>
         </is>
       </c>
-      <c r="BA1" s="2" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>WhatsApp_Message</t>
         </is>
       </c>
-      <c r="BB1" s="2" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>QR_Code_URL</t>
         </is>
       </c>
-      <c r="BC1" s="2" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Print_Status</t>
         </is>
       </c>
-      <c r="BD1" s="2" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Print_Slot</t>
         </is>
       </c>
-      <c r="BE1" s="2" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>FB_Posted_Date</t>
         </is>
       </c>
-      <c r="BF1" s="2" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>FB_Post_Link</t>
         </is>
       </c>
-      <c r="BG1" s="2" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Website_Listed</t>
         </is>
       </c>
-      <c r="BH1" s="2" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Website_URL</t>
         </is>
       </c>
-      <c r="BI1" s="2" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Marketing_Priority</t>
         </is>
       </c>
-      <c r="BJ1" s="2" t="inlineStr">
+      <c r="BJ1" s="3" t="inlineStr">
         <is>
           <t>Total_Units</t>
         </is>
       </c>
-      <c r="BK1" s="2" t="inlineStr">
+      <c r="BK1" s="3" t="inlineStr">
         <is>
           <t>Units_Available</t>
         </is>
       </c>
-      <c r="BL1" s="2" t="inlineStr">
+      <c r="BL1" s="3" t="inlineStr">
         <is>
           <t>Transfer_Date</t>
         </is>
       </c>
-      <c r="BM1" s="2" t="inlineStr">
+      <c r="BM1" s="3" t="inlineStr">
         <is>
           <t>Payment_Plan</t>
         </is>
       </c>
-      <c r="BN1" s="2" t="inlineStr">
+      <c r="BN1" s="3" t="inlineStr">
         <is>
           <t>Installment_Available</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="18">
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Available,Reserved,Sold,Rented,Pending,Off Market"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Project,Resale,Rental-LT,Rental-ST"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Condo,Villa,House,Townhouse,Land,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Pattaya City,Jomtien,Na Jomtien,Pratumnak,Wongamat,Bang Saray,Huay Yai,East Pattaya,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"THB,USD,EUR"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Freehold,Leasehold,Company"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No,N/A"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Unfurnished,Partly Furnished,Fully Furnished"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AC2:AC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"New,Excellent,Good,Fair,Needs Renovation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AM2:AM1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Owner Direct,Agent,LINE Group,Facebook,Website,Walk-in,Referral"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AO2:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Somchai S.,Napat K.,John D.,Sarah M.,Unassigned"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AP2:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AQ2:AQ1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AR2:AR1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BC2:BC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BG2:BG1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BI2:BI1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1483,335 +1605,454 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="15" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="30" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
+    <col width="12" customWidth="1" min="30" max="30"/>
+    <col width="12" customWidth="1" min="31" max="31"/>
+    <col width="15" customWidth="1" min="32" max="32"/>
+    <col width="20" customWidth="1" min="33" max="33"/>
+    <col width="15" customWidth="1" min="34" max="34"/>
+    <col width="15" customWidth="1" min="35" max="35"/>
+    <col width="15" customWidth="1" min="36" max="36"/>
+    <col width="15" customWidth="1" min="37" max="37"/>
+    <col width="15" customWidth="1" min="38" max="38"/>
+    <col width="15" customWidth="1" min="39" max="39"/>
+    <col width="25" customWidth="1" min="40" max="40"/>
+    <col width="15" customWidth="1" min="41" max="41"/>
+    <col width="12" customWidth="1" min="42" max="42"/>
+    <col width="12" customWidth="1" min="43" max="43"/>
+    <col width="12" customWidth="1" min="44" max="44"/>
+    <col width="12" customWidth="1" min="45" max="45"/>
+    <col width="12" customWidth="1" min="46" max="46"/>
+    <col width="12" customWidth="1" min="47" max="47"/>
+    <col width="12" customWidth="1" min="48" max="48"/>
+    <col width="12" customWidth="1" min="49" max="49"/>
+    <col width="30" customWidth="1" min="50" max="50"/>
+    <col width="20" customWidth="1" min="51" max="51"/>
+    <col width="12" customWidth="1" min="52" max="52"/>
+    <col width="40" customWidth="1" min="53" max="53"/>
+    <col width="40" customWidth="1" min="54" max="54"/>
+    <col width="12" customWidth="1" min="55" max="55"/>
+    <col width="10" customWidth="1" min="56" max="56"/>
+    <col width="12" customWidth="1" min="57" max="57"/>
+    <col width="15" customWidth="1" min="58" max="58"/>
+    <col width="12" customWidth="1" min="59" max="59"/>
+    <col width="15" customWidth="1" min="60" max="60"/>
+    <col width="15" customWidth="1" min="61" max="61"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Property_ID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Project_Name</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Unit_Number</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Location_Area</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Location_Sub</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Latitude</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Longitude</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Price_Sale</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Price_Rent</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="O1" s="2" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Price_Per_SQM</t>
         </is>
       </c>
-      <c r="P1" s="2" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Negotiable</t>
         </is>
       </c>
-      <c r="Q1" s="2" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Commission_Rate</t>
         </is>
       </c>
-      <c r="R1" s="2" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Owner_Type</t>
         </is>
       </c>
-      <c r="S1" s="2" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Foreign_Quota</t>
         </is>
       </c>
-      <c r="T1" s="2" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Bedrooms</t>
         </is>
       </c>
-      <c r="U1" s="2" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Bathrooms</t>
         </is>
       </c>
-      <c r="V1" s="2" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Size_SQM</t>
         </is>
       </c>
-      <c r="W1" s="2" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Size_SQW</t>
         </is>
       </c>
-      <c r="X1" s="2" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Floor_Level</t>
         </is>
       </c>
-      <c r="Y1" s="2" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>View</t>
         </is>
       </c>
-      <c r="Z1" s="2" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Furnishing</t>
         </is>
       </c>
-      <c r="AA1" s="2" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Parking</t>
         </is>
       </c>
-      <c r="AB1" s="2" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Facilities</t>
         </is>
       </c>
-      <c r="AC1" s="2" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Condition</t>
         </is>
       </c>
-      <c r="AD1" s="2" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Year_Built</t>
         </is>
       </c>
-      <c r="AE1" s="2" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Year_Renovated</t>
         </is>
       </c>
-      <c r="AF1" s="2" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Title_Deed</t>
         </is>
       </c>
-      <c r="AG1" s="2" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Developer</t>
         </is>
       </c>
-      <c r="AH1" s="2" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Photos_Link</t>
         </is>
       </c>
-      <c r="AI1" s="2" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Video_Link</t>
         </is>
       </c>
-      <c r="AJ1" s="2" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Brochure_Link</t>
         </is>
       </c>
-      <c r="AK1" s="2" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Virtual_Tour</t>
         </is>
       </c>
-      <c r="AL1" s="2" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Listing_URL</t>
         </is>
       </c>
-      <c r="AM1" s="2" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="AN1" s="2" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Source_Contact</t>
         </is>
       </c>
-      <c r="AO1" s="2" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Assigned_Agent</t>
         </is>
       </c>
-      <c r="AP1" s="2" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="AQ1" s="2" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Featured</t>
         </is>
       </c>
-      <c r="AR1" s="2" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Active_Marketing</t>
         </is>
       </c>
-      <c r="AS1" s="2" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Date_Added</t>
         </is>
       </c>
-      <c r="AT1" s="2" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Date_Updated</t>
         </is>
       </c>
-      <c r="AU1" s="2" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Date_Available</t>
         </is>
       </c>
-      <c r="AV1" s="2" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Views_Count</t>
         </is>
       </c>
-      <c r="AW1" s="2" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Viewings_Count</t>
         </is>
       </c>
-      <c r="AX1" s="2" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Notes_Internal</t>
         </is>
       </c>
-      <c r="AY1" s="2" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Tags</t>
         </is>
       </c>
-      <c r="AZ1" s="2" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Language</t>
         </is>
       </c>
-      <c r="BA1" s="2" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>WhatsApp_Message</t>
         </is>
       </c>
-      <c r="BB1" s="2" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>QR_Code_URL</t>
         </is>
       </c>
-      <c r="BC1" s="2" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Print_Status</t>
         </is>
       </c>
-      <c r="BD1" s="2" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Print_Slot</t>
         </is>
       </c>
-      <c r="BE1" s="2" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>FB_Posted_Date</t>
         </is>
       </c>
-      <c r="BF1" s="2" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>FB_Post_Link</t>
         </is>
       </c>
-      <c r="BG1" s="2" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Website_Listed</t>
         </is>
       </c>
-      <c r="BH1" s="2" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Website_URL</t>
         </is>
       </c>
-      <c r="BI1" s="2" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Marketing_Priority</t>
         </is>
       </c>
-      <c r="BJ1" s="2" t="inlineStr">
+      <c r="BJ1" s="3" t="inlineStr">
         <is>
           <t>Owner_Contact</t>
         </is>
       </c>
-      <c r="BK1" s="2" t="inlineStr">
+      <c r="BK1" s="3" t="inlineStr">
         <is>
           <t>Reason_Selling</t>
         </is>
       </c>
-      <c r="BL1" s="2" t="inlineStr">
+      <c r="BL1" s="3" t="inlineStr">
         <is>
           <t>Occupancy</t>
         </is>
       </c>
-      <c r="BM1" s="2" t="inlineStr">
+      <c r="BM1" s="3" t="inlineStr">
         <is>
           <t>Flexibility</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="18">
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Available,Reserved,Sold,Rented,Pending,Off Market"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Project,Resale,Rental-LT,Rental-ST"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Condo,Villa,House,Townhouse,Land,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Pattaya City,Jomtien,Na Jomtien,Pratumnak,Wongamat,Bang Saray,Huay Yai,East Pattaya,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"THB,USD,EUR"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Freehold,Leasehold,Company"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No,N/A"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Unfurnished,Partly Furnished,Fully Furnished"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AC2:AC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"New,Excellent,Good,Fair,Needs Renovation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AM2:AM1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Owner Direct,Agent,LINE Group,Facebook,Website,Walk-in,Referral"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AO2:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Somchai S.,Napat K.,John D.,Sarah M.,Unassigned"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AP2:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AQ2:AQ1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AR2:AR1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BC2:BC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BG2:BG1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BI2:BI1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1832,335 +2073,454 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="15" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="30" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
+    <col width="12" customWidth="1" min="30" max="30"/>
+    <col width="12" customWidth="1" min="31" max="31"/>
+    <col width="15" customWidth="1" min="32" max="32"/>
+    <col width="20" customWidth="1" min="33" max="33"/>
+    <col width="15" customWidth="1" min="34" max="34"/>
+    <col width="15" customWidth="1" min="35" max="35"/>
+    <col width="15" customWidth="1" min="36" max="36"/>
+    <col width="15" customWidth="1" min="37" max="37"/>
+    <col width="15" customWidth="1" min="38" max="38"/>
+    <col width="15" customWidth="1" min="39" max="39"/>
+    <col width="25" customWidth="1" min="40" max="40"/>
+    <col width="15" customWidth="1" min="41" max="41"/>
+    <col width="12" customWidth="1" min="42" max="42"/>
+    <col width="12" customWidth="1" min="43" max="43"/>
+    <col width="12" customWidth="1" min="44" max="44"/>
+    <col width="12" customWidth="1" min="45" max="45"/>
+    <col width="12" customWidth="1" min="46" max="46"/>
+    <col width="12" customWidth="1" min="47" max="47"/>
+    <col width="12" customWidth="1" min="48" max="48"/>
+    <col width="12" customWidth="1" min="49" max="49"/>
+    <col width="30" customWidth="1" min="50" max="50"/>
+    <col width="20" customWidth="1" min="51" max="51"/>
+    <col width="12" customWidth="1" min="52" max="52"/>
+    <col width="40" customWidth="1" min="53" max="53"/>
+    <col width="40" customWidth="1" min="54" max="54"/>
+    <col width="12" customWidth="1" min="55" max="55"/>
+    <col width="10" customWidth="1" min="56" max="56"/>
+    <col width="12" customWidth="1" min="57" max="57"/>
+    <col width="15" customWidth="1" min="58" max="58"/>
+    <col width="12" customWidth="1" min="59" max="59"/>
+    <col width="15" customWidth="1" min="60" max="60"/>
+    <col width="15" customWidth="1" min="61" max="61"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Property_ID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Project_Name</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Unit_Number</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Location_Area</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Location_Sub</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Latitude</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Longitude</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Price_Sale</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Price_Rent</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="O1" s="2" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Price_Per_SQM</t>
         </is>
       </c>
-      <c r="P1" s="2" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Negotiable</t>
         </is>
       </c>
-      <c r="Q1" s="2" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Commission_Rate</t>
         </is>
       </c>
-      <c r="R1" s="2" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Owner_Type</t>
         </is>
       </c>
-      <c r="S1" s="2" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Foreign_Quota</t>
         </is>
       </c>
-      <c r="T1" s="2" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Bedrooms</t>
         </is>
       </c>
-      <c r="U1" s="2" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Bathrooms</t>
         </is>
       </c>
-      <c r="V1" s="2" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Size_SQM</t>
         </is>
       </c>
-      <c r="W1" s="2" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Size_SQW</t>
         </is>
       </c>
-      <c r="X1" s="2" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Floor_Level</t>
         </is>
       </c>
-      <c r="Y1" s="2" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>View</t>
         </is>
       </c>
-      <c r="Z1" s="2" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Furnishing</t>
         </is>
       </c>
-      <c r="AA1" s="2" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Parking</t>
         </is>
       </c>
-      <c r="AB1" s="2" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Facilities</t>
         </is>
       </c>
-      <c r="AC1" s="2" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Condition</t>
         </is>
       </c>
-      <c r="AD1" s="2" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Year_Built</t>
         </is>
       </c>
-      <c r="AE1" s="2" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Year_Renovated</t>
         </is>
       </c>
-      <c r="AF1" s="2" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Title_Deed</t>
         </is>
       </c>
-      <c r="AG1" s="2" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Developer</t>
         </is>
       </c>
-      <c r="AH1" s="2" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Photos_Link</t>
         </is>
       </c>
-      <c r="AI1" s="2" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Video_Link</t>
         </is>
       </c>
-      <c r="AJ1" s="2" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Brochure_Link</t>
         </is>
       </c>
-      <c r="AK1" s="2" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Virtual_Tour</t>
         </is>
       </c>
-      <c r="AL1" s="2" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Listing_URL</t>
         </is>
       </c>
-      <c r="AM1" s="2" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="AN1" s="2" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Source_Contact</t>
         </is>
       </c>
-      <c r="AO1" s="2" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Assigned_Agent</t>
         </is>
       </c>
-      <c r="AP1" s="2" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="AQ1" s="2" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Featured</t>
         </is>
       </c>
-      <c r="AR1" s="2" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Active_Marketing</t>
         </is>
       </c>
-      <c r="AS1" s="2" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Date_Added</t>
         </is>
       </c>
-      <c r="AT1" s="2" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Date_Updated</t>
         </is>
       </c>
-      <c r="AU1" s="2" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Date_Available</t>
         </is>
       </c>
-      <c r="AV1" s="2" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Views_Count</t>
         </is>
       </c>
-      <c r="AW1" s="2" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Viewings_Count</t>
         </is>
       </c>
-      <c r="AX1" s="2" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Notes_Internal</t>
         </is>
       </c>
-      <c r="AY1" s="2" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Tags</t>
         </is>
       </c>
-      <c r="AZ1" s="2" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Language</t>
         </is>
       </c>
-      <c r="BA1" s="2" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>WhatsApp_Message</t>
         </is>
       </c>
-      <c r="BB1" s="2" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>QR_Code_URL</t>
         </is>
       </c>
-      <c r="BC1" s="2" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Print_Status</t>
         </is>
       </c>
-      <c r="BD1" s="2" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Print_Slot</t>
         </is>
       </c>
-      <c r="BE1" s="2" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>FB_Posted_Date</t>
         </is>
       </c>
-      <c r="BF1" s="2" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>FB_Post_Link</t>
         </is>
       </c>
-      <c r="BG1" s="2" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Website_Listed</t>
         </is>
       </c>
-      <c r="BH1" s="2" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Website_URL</t>
         </is>
       </c>
-      <c r="BI1" s="2" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Marketing_Priority</t>
         </is>
       </c>
-      <c r="BJ1" s="2" t="inlineStr">
+      <c r="BJ1" s="3" t="inlineStr">
         <is>
           <t>Min_Contract</t>
         </is>
       </c>
-      <c r="BK1" s="2" t="inlineStr">
+      <c r="BK1" s="3" t="inlineStr">
         <is>
           <t>Utilities_Included</t>
         </is>
       </c>
-      <c r="BL1" s="2" t="inlineStr">
+      <c r="BL1" s="3" t="inlineStr">
         <is>
           <t>Pets_Allowed</t>
         </is>
       </c>
-      <c r="BM1" s="2" t="inlineStr">
+      <c r="BM1" s="3" t="inlineStr">
         <is>
           <t>Available_From</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="18">
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Available,Reserved,Sold,Rented,Pending,Off Market"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Project,Resale,Rental-LT,Rental-ST"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Condo,Villa,House,Townhouse,Land,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Pattaya City,Jomtien,Na Jomtien,Pratumnak,Wongamat,Bang Saray,Huay Yai,East Pattaya,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"THB,USD,EUR"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Freehold,Leasehold,Company"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No,N/A"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Unfurnished,Partly Furnished,Fully Furnished"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AC2:AC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"New,Excellent,Good,Fair,Needs Renovation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AM2:AM1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Owner Direct,Agent,LINE Group,Facebook,Website,Walk-in,Referral"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AO2:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Somchai S.,Napat K.,John D.,Sarah M.,Unassigned"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AP2:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AQ2:AQ1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AR2:AR1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BC2:BC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BG2:BG1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BI2:BI1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2181,340 +2541,459 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="15" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="30" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
+    <col width="12" customWidth="1" min="30" max="30"/>
+    <col width="12" customWidth="1" min="31" max="31"/>
+    <col width="15" customWidth="1" min="32" max="32"/>
+    <col width="20" customWidth="1" min="33" max="33"/>
+    <col width="15" customWidth="1" min="34" max="34"/>
+    <col width="15" customWidth="1" min="35" max="35"/>
+    <col width="15" customWidth="1" min="36" max="36"/>
+    <col width="15" customWidth="1" min="37" max="37"/>
+    <col width="15" customWidth="1" min="38" max="38"/>
+    <col width="15" customWidth="1" min="39" max="39"/>
+    <col width="25" customWidth="1" min="40" max="40"/>
+    <col width="15" customWidth="1" min="41" max="41"/>
+    <col width="12" customWidth="1" min="42" max="42"/>
+    <col width="12" customWidth="1" min="43" max="43"/>
+    <col width="12" customWidth="1" min="44" max="44"/>
+    <col width="12" customWidth="1" min="45" max="45"/>
+    <col width="12" customWidth="1" min="46" max="46"/>
+    <col width="12" customWidth="1" min="47" max="47"/>
+    <col width="12" customWidth="1" min="48" max="48"/>
+    <col width="12" customWidth="1" min="49" max="49"/>
+    <col width="30" customWidth="1" min="50" max="50"/>
+    <col width="20" customWidth="1" min="51" max="51"/>
+    <col width="12" customWidth="1" min="52" max="52"/>
+    <col width="40" customWidth="1" min="53" max="53"/>
+    <col width="40" customWidth="1" min="54" max="54"/>
+    <col width="12" customWidth="1" min="55" max="55"/>
+    <col width="10" customWidth="1" min="56" max="56"/>
+    <col width="12" customWidth="1" min="57" max="57"/>
+    <col width="15" customWidth="1" min="58" max="58"/>
+    <col width="12" customWidth="1" min="59" max="59"/>
+    <col width="15" customWidth="1" min="60" max="60"/>
+    <col width="15" customWidth="1" min="61" max="61"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Property_ID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Project_Name</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Unit_Number</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Location_Area</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Location_Sub</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Latitude</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Longitude</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Price_Sale</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Price_Rent</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="O1" s="2" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Price_Per_SQM</t>
         </is>
       </c>
-      <c r="P1" s="2" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Negotiable</t>
         </is>
       </c>
-      <c r="Q1" s="2" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Commission_Rate</t>
         </is>
       </c>
-      <c r="R1" s="2" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Owner_Type</t>
         </is>
       </c>
-      <c r="S1" s="2" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Foreign_Quota</t>
         </is>
       </c>
-      <c r="T1" s="2" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Bedrooms</t>
         </is>
       </c>
-      <c r="U1" s="2" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Bathrooms</t>
         </is>
       </c>
-      <c r="V1" s="2" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Size_SQM</t>
         </is>
       </c>
-      <c r="W1" s="2" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Size_SQW</t>
         </is>
       </c>
-      <c r="X1" s="2" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Floor_Level</t>
         </is>
       </c>
-      <c r="Y1" s="2" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>View</t>
         </is>
       </c>
-      <c r="Z1" s="2" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Furnishing</t>
         </is>
       </c>
-      <c r="AA1" s="2" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Parking</t>
         </is>
       </c>
-      <c r="AB1" s="2" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Facilities</t>
         </is>
       </c>
-      <c r="AC1" s="2" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Condition</t>
         </is>
       </c>
-      <c r="AD1" s="2" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Year_Built</t>
         </is>
       </c>
-      <c r="AE1" s="2" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Year_Renovated</t>
         </is>
       </c>
-      <c r="AF1" s="2" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Title_Deed</t>
         </is>
       </c>
-      <c r="AG1" s="2" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Developer</t>
         </is>
       </c>
-      <c r="AH1" s="2" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Photos_Link</t>
         </is>
       </c>
-      <c r="AI1" s="2" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Video_Link</t>
         </is>
       </c>
-      <c r="AJ1" s="2" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Brochure_Link</t>
         </is>
       </c>
-      <c r="AK1" s="2" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Virtual_Tour</t>
         </is>
       </c>
-      <c r="AL1" s="2" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Listing_URL</t>
         </is>
       </c>
-      <c r="AM1" s="2" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="AN1" s="2" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Source_Contact</t>
         </is>
       </c>
-      <c r="AO1" s="2" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Assigned_Agent</t>
         </is>
       </c>
-      <c r="AP1" s="2" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="AQ1" s="2" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Featured</t>
         </is>
       </c>
-      <c r="AR1" s="2" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Active_Marketing</t>
         </is>
       </c>
-      <c r="AS1" s="2" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Date_Added</t>
         </is>
       </c>
-      <c r="AT1" s="2" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Date_Updated</t>
         </is>
       </c>
-      <c r="AU1" s="2" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Date_Available</t>
         </is>
       </c>
-      <c r="AV1" s="2" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Views_Count</t>
         </is>
       </c>
-      <c r="AW1" s="2" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Viewings_Count</t>
         </is>
       </c>
-      <c r="AX1" s="2" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Notes_Internal</t>
         </is>
       </c>
-      <c r="AY1" s="2" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Tags</t>
         </is>
       </c>
-      <c r="AZ1" s="2" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Language</t>
         </is>
       </c>
-      <c r="BA1" s="2" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>WhatsApp_Message</t>
         </is>
       </c>
-      <c r="BB1" s="2" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>QR_Code_URL</t>
         </is>
       </c>
-      <c r="BC1" s="2" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Print_Status</t>
         </is>
       </c>
-      <c r="BD1" s="2" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Print_Slot</t>
         </is>
       </c>
-      <c r="BE1" s="2" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>FB_Posted_Date</t>
         </is>
       </c>
-      <c r="BF1" s="2" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>FB_Post_Link</t>
         </is>
       </c>
-      <c r="BG1" s="2" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Website_Listed</t>
         </is>
       </c>
-      <c r="BH1" s="2" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Website_URL</t>
         </is>
       </c>
-      <c r="BI1" s="2" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Marketing_Priority</t>
         </is>
       </c>
-      <c r="BJ1" s="2" t="inlineStr">
+      <c r="BJ1" s="3" t="inlineStr">
         <is>
           <t>Min_Nights</t>
         </is>
       </c>
-      <c r="BK1" s="2" t="inlineStr">
+      <c r="BK1" s="3" t="inlineStr">
         <is>
           <t>Price_High_Season</t>
         </is>
       </c>
-      <c r="BL1" s="2" t="inlineStr">
+      <c r="BL1" s="3" t="inlineStr">
         <is>
           <t>Price_Low_Season</t>
         </is>
       </c>
-      <c r="BM1" s="2" t="inlineStr">
+      <c r="BM1" s="3" t="inlineStr">
         <is>
           <t>Cleaning_Fee</t>
         </is>
       </c>
-      <c r="BN1" s="2" t="inlineStr">
+      <c r="BN1" s="3" t="inlineStr">
         <is>
           <t>Booking_Platforms</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="18">
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Available,Reserved,Sold,Rented,Pending,Off Market"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Project,Resale,Rental-LT,Rental-ST"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Condo,Villa,House,Townhouse,Land,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Pattaya City,Jomtien,Na Jomtien,Pratumnak,Wongamat,Bang Saray,Huay Yai,East Pattaya,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"THB,USD,EUR"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Freehold,Leasehold,Company"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No,N/A"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Unfurnished,Partly Furnished,Fully Furnished"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AC2:AC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"New,Excellent,Good,Fair,Needs Renovation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AM2:AM1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Owner Direct,Agent,LINE Group,Facebook,Website,Walk-in,Referral"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AO2:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Somchai S.,Napat K.,John D.,Sarah M.,Unassigned"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AP2:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AQ2:AQ1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AR2:AR1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BC2:BC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BG2:BG1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BI2:BI1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2535,315 +3014,434 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="15" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="30" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
+    <col width="12" customWidth="1" min="30" max="30"/>
+    <col width="12" customWidth="1" min="31" max="31"/>
+    <col width="15" customWidth="1" min="32" max="32"/>
+    <col width="20" customWidth="1" min="33" max="33"/>
+    <col width="15" customWidth="1" min="34" max="34"/>
+    <col width="15" customWidth="1" min="35" max="35"/>
+    <col width="15" customWidth="1" min="36" max="36"/>
+    <col width="15" customWidth="1" min="37" max="37"/>
+    <col width="15" customWidth="1" min="38" max="38"/>
+    <col width="15" customWidth="1" min="39" max="39"/>
+    <col width="25" customWidth="1" min="40" max="40"/>
+    <col width="15" customWidth="1" min="41" max="41"/>
+    <col width="12" customWidth="1" min="42" max="42"/>
+    <col width="12" customWidth="1" min="43" max="43"/>
+    <col width="12" customWidth="1" min="44" max="44"/>
+    <col width="12" customWidth="1" min="45" max="45"/>
+    <col width="12" customWidth="1" min="46" max="46"/>
+    <col width="12" customWidth="1" min="47" max="47"/>
+    <col width="12" customWidth="1" min="48" max="48"/>
+    <col width="12" customWidth="1" min="49" max="49"/>
+    <col width="30" customWidth="1" min="50" max="50"/>
+    <col width="20" customWidth="1" min="51" max="51"/>
+    <col width="12" customWidth="1" min="52" max="52"/>
+    <col width="40" customWidth="1" min="53" max="53"/>
+    <col width="40" customWidth="1" min="54" max="54"/>
+    <col width="12" customWidth="1" min="55" max="55"/>
+    <col width="10" customWidth="1" min="56" max="56"/>
+    <col width="12" customWidth="1" min="57" max="57"/>
+    <col width="15" customWidth="1" min="58" max="58"/>
+    <col width="12" customWidth="1" min="59" max="59"/>
+    <col width="15" customWidth="1" min="60" max="60"/>
+    <col width="15" customWidth="1" min="61" max="61"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Property_ID</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Project_Name</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>Unit_Number</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Location_Area</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>Location_Sub</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>Latitude</t>
         </is>
       </c>
-      <c r="K1" s="3" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>Longitude</t>
         </is>
       </c>
-      <c r="L1" s="3" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>Price_Sale</t>
         </is>
       </c>
-      <c r="M1" s="3" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>Price_Rent</t>
         </is>
       </c>
-      <c r="N1" s="3" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="O1" s="3" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>Price_Per_SQM</t>
         </is>
       </c>
-      <c r="P1" s="3" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>Negotiable</t>
         </is>
       </c>
-      <c r="Q1" s="3" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>Commission_Rate</t>
         </is>
       </c>
-      <c r="R1" s="3" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>Owner_Type</t>
         </is>
       </c>
-      <c r="S1" s="3" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>Foreign_Quota</t>
         </is>
       </c>
-      <c r="T1" s="3" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>Bedrooms</t>
         </is>
       </c>
-      <c r="U1" s="3" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>Bathrooms</t>
         </is>
       </c>
-      <c r="V1" s="3" t="inlineStr">
+      <c r="V1" s="4" t="inlineStr">
         <is>
           <t>Size_SQM</t>
         </is>
       </c>
-      <c r="W1" s="3" t="inlineStr">
+      <c r="W1" s="4" t="inlineStr">
         <is>
           <t>Size_SQW</t>
         </is>
       </c>
-      <c r="X1" s="3" t="inlineStr">
+      <c r="X1" s="4" t="inlineStr">
         <is>
           <t>Floor_Level</t>
         </is>
       </c>
-      <c r="Y1" s="3" t="inlineStr">
+      <c r="Y1" s="4" t="inlineStr">
         <is>
           <t>View</t>
         </is>
       </c>
-      <c r="Z1" s="3" t="inlineStr">
+      <c r="Z1" s="4" t="inlineStr">
         <is>
           <t>Furnishing</t>
         </is>
       </c>
-      <c r="AA1" s="3" t="inlineStr">
+      <c r="AA1" s="4" t="inlineStr">
         <is>
           <t>Parking</t>
         </is>
       </c>
-      <c r="AB1" s="3" t="inlineStr">
+      <c r="AB1" s="4" t="inlineStr">
         <is>
           <t>Facilities</t>
         </is>
       </c>
-      <c r="AC1" s="3" t="inlineStr">
+      <c r="AC1" s="4" t="inlineStr">
         <is>
           <t>Condition</t>
         </is>
       </c>
-      <c r="AD1" s="3" t="inlineStr">
+      <c r="AD1" s="4" t="inlineStr">
         <is>
           <t>Year_Built</t>
         </is>
       </c>
-      <c r="AE1" s="3" t="inlineStr">
+      <c r="AE1" s="4" t="inlineStr">
         <is>
           <t>Year_Renovated</t>
         </is>
       </c>
-      <c r="AF1" s="3" t="inlineStr">
+      <c r="AF1" s="4" t="inlineStr">
         <is>
           <t>Title_Deed</t>
         </is>
       </c>
-      <c r="AG1" s="3" t="inlineStr">
+      <c r="AG1" s="4" t="inlineStr">
         <is>
           <t>Developer</t>
         </is>
       </c>
-      <c r="AH1" s="3" t="inlineStr">
+      <c r="AH1" s="4" t="inlineStr">
         <is>
           <t>Photos_Link</t>
         </is>
       </c>
-      <c r="AI1" s="3" t="inlineStr">
+      <c r="AI1" s="4" t="inlineStr">
         <is>
           <t>Video_Link</t>
         </is>
       </c>
-      <c r="AJ1" s="3" t="inlineStr">
+      <c r="AJ1" s="4" t="inlineStr">
         <is>
           <t>Brochure_Link</t>
         </is>
       </c>
-      <c r="AK1" s="3" t="inlineStr">
+      <c r="AK1" s="4" t="inlineStr">
         <is>
           <t>Virtual_Tour</t>
         </is>
       </c>
-      <c r="AL1" s="3" t="inlineStr">
+      <c r="AL1" s="4" t="inlineStr">
         <is>
           <t>Listing_URL</t>
         </is>
       </c>
-      <c r="AM1" s="3" t="inlineStr">
+      <c r="AM1" s="4" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="AN1" s="3" t="inlineStr">
+      <c r="AN1" s="4" t="inlineStr">
         <is>
           <t>Source_Contact</t>
         </is>
       </c>
-      <c r="AO1" s="3" t="inlineStr">
+      <c r="AO1" s="4" t="inlineStr">
         <is>
           <t>Assigned_Agent</t>
         </is>
       </c>
-      <c r="AP1" s="3" t="inlineStr">
+      <c r="AP1" s="4" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="AQ1" s="3" t="inlineStr">
+      <c r="AQ1" s="4" t="inlineStr">
         <is>
           <t>Featured</t>
         </is>
       </c>
-      <c r="AR1" s="3" t="inlineStr">
+      <c r="AR1" s="4" t="inlineStr">
         <is>
           <t>Active_Marketing</t>
         </is>
       </c>
-      <c r="AS1" s="3" t="inlineStr">
+      <c r="AS1" s="4" t="inlineStr">
         <is>
           <t>Date_Added</t>
         </is>
       </c>
-      <c r="AT1" s="3" t="inlineStr">
+      <c r="AT1" s="4" t="inlineStr">
         <is>
           <t>Date_Updated</t>
         </is>
       </c>
-      <c r="AU1" s="3" t="inlineStr">
+      <c r="AU1" s="4" t="inlineStr">
         <is>
           <t>Date_Available</t>
         </is>
       </c>
-      <c r="AV1" s="3" t="inlineStr">
+      <c r="AV1" s="4" t="inlineStr">
         <is>
           <t>Views_Count</t>
         </is>
       </c>
-      <c r="AW1" s="3" t="inlineStr">
+      <c r="AW1" s="4" t="inlineStr">
         <is>
           <t>Viewings_Count</t>
         </is>
       </c>
-      <c r="AX1" s="3" t="inlineStr">
+      <c r="AX1" s="4" t="inlineStr">
         <is>
           <t>Notes_Internal</t>
         </is>
       </c>
-      <c r="AY1" s="3" t="inlineStr">
+      <c r="AY1" s="4" t="inlineStr">
         <is>
           <t>Tags</t>
         </is>
       </c>
-      <c r="AZ1" s="3" t="inlineStr">
+      <c r="AZ1" s="4" t="inlineStr">
         <is>
           <t>Language</t>
         </is>
       </c>
-      <c r="BA1" s="3" t="inlineStr">
+      <c r="BA1" s="4" t="inlineStr">
         <is>
           <t>WhatsApp_Message</t>
         </is>
       </c>
-      <c r="BB1" s="3" t="inlineStr">
+      <c r="BB1" s="4" t="inlineStr">
         <is>
           <t>QR_Code_URL</t>
         </is>
       </c>
-      <c r="BC1" s="3" t="inlineStr">
+      <c r="BC1" s="4" t="inlineStr">
         <is>
           <t>Print_Status</t>
         </is>
       </c>
-      <c r="BD1" s="3" t="inlineStr">
+      <c r="BD1" s="4" t="inlineStr">
         <is>
           <t>Print_Slot</t>
         </is>
       </c>
-      <c r="BE1" s="3" t="inlineStr">
+      <c r="BE1" s="4" t="inlineStr">
         <is>
           <t>FB_Posted_Date</t>
         </is>
       </c>
-      <c r="BF1" s="3" t="inlineStr">
+      <c r="BF1" s="4" t="inlineStr">
         <is>
           <t>FB_Post_Link</t>
         </is>
       </c>
-      <c r="BG1" s="3" t="inlineStr">
+      <c r="BG1" s="4" t="inlineStr">
         <is>
           <t>Website_Listed</t>
         </is>
       </c>
-      <c r="BH1" s="3" t="inlineStr">
+      <c r="BH1" s="4" t="inlineStr">
         <is>
           <t>Website_URL</t>
         </is>
       </c>
-      <c r="BI1" s="3" t="inlineStr">
+      <c r="BI1" s="4" t="inlineStr">
         <is>
           <t>Marketing_Priority</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="18">
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Available,Reserved,Sold,Rented,Pending,Off Market"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Project,Resale,Rental-LT,Rental-ST"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Condo,Villa,House,Townhouse,Land,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Pattaya City,Jomtien,Na Jomtien,Pratumnak,Wongamat,Bang Saray,Huay Yai,East Pattaya,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"THB,USD,EUR"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Freehold,Leasehold,Company"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No,N/A"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Unfurnished,Partly Furnished,Fully Furnished"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AC2:AC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"New,Excellent,Good,Fair,Needs Renovation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AM2:AM1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Owner Direct,Agent,LINE Group,Facebook,Website,Walk-in,Referral"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AO2:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Somchai S.,Napat K.,John D.,Sarah M.,Unassigned"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AP2:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AQ2:AQ1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AR2:AR1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BC2:BC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BG2:BG1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BI2:BI1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2864,315 +3462,434 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="15" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="30" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
+    <col width="12" customWidth="1" min="30" max="30"/>
+    <col width="12" customWidth="1" min="31" max="31"/>
+    <col width="15" customWidth="1" min="32" max="32"/>
+    <col width="20" customWidth="1" min="33" max="33"/>
+    <col width="15" customWidth="1" min="34" max="34"/>
+    <col width="15" customWidth="1" min="35" max="35"/>
+    <col width="15" customWidth="1" min="36" max="36"/>
+    <col width="15" customWidth="1" min="37" max="37"/>
+    <col width="15" customWidth="1" min="38" max="38"/>
+    <col width="15" customWidth="1" min="39" max="39"/>
+    <col width="25" customWidth="1" min="40" max="40"/>
+    <col width="15" customWidth="1" min="41" max="41"/>
+    <col width="12" customWidth="1" min="42" max="42"/>
+    <col width="12" customWidth="1" min="43" max="43"/>
+    <col width="12" customWidth="1" min="44" max="44"/>
+    <col width="12" customWidth="1" min="45" max="45"/>
+    <col width="12" customWidth="1" min="46" max="46"/>
+    <col width="12" customWidth="1" min="47" max="47"/>
+    <col width="12" customWidth="1" min="48" max="48"/>
+    <col width="12" customWidth="1" min="49" max="49"/>
+    <col width="30" customWidth="1" min="50" max="50"/>
+    <col width="20" customWidth="1" min="51" max="51"/>
+    <col width="12" customWidth="1" min="52" max="52"/>
+    <col width="40" customWidth="1" min="53" max="53"/>
+    <col width="40" customWidth="1" min="54" max="54"/>
+    <col width="12" customWidth="1" min="55" max="55"/>
+    <col width="10" customWidth="1" min="56" max="56"/>
+    <col width="12" customWidth="1" min="57" max="57"/>
+    <col width="15" customWidth="1" min="58" max="58"/>
+    <col width="12" customWidth="1" min="59" max="59"/>
+    <col width="15" customWidth="1" min="60" max="60"/>
+    <col width="15" customWidth="1" min="61" max="61"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Property_ID</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Project_Name</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Unit_Number</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Location_Area</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>Location_Sub</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>Latitude</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>Longitude</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>Price_Sale</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="M1" s="5" t="inlineStr">
         <is>
           <t>Price_Rent</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="N1" s="5" t="inlineStr">
         <is>
           <t>Currency</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="O1" s="5" t="inlineStr">
         <is>
           <t>Price_Per_SQM</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="P1" s="5" t="inlineStr">
         <is>
           <t>Negotiable</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="Q1" s="5" t="inlineStr">
         <is>
           <t>Commission_Rate</t>
         </is>
       </c>
-      <c r="R1" s="4" t="inlineStr">
+      <c r="R1" s="5" t="inlineStr">
         <is>
           <t>Owner_Type</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
+      <c r="S1" s="5" t="inlineStr">
         <is>
           <t>Foreign_Quota</t>
         </is>
       </c>
-      <c r="T1" s="4" t="inlineStr">
+      <c r="T1" s="5" t="inlineStr">
         <is>
           <t>Bedrooms</t>
         </is>
       </c>
-      <c r="U1" s="4" t="inlineStr">
+      <c r="U1" s="5" t="inlineStr">
         <is>
           <t>Bathrooms</t>
         </is>
       </c>
-      <c r="V1" s="4" t="inlineStr">
+      <c r="V1" s="5" t="inlineStr">
         <is>
           <t>Size_SQM</t>
         </is>
       </c>
-      <c r="W1" s="4" t="inlineStr">
+      <c r="W1" s="5" t="inlineStr">
         <is>
           <t>Size_SQW</t>
         </is>
       </c>
-      <c r="X1" s="4" t="inlineStr">
+      <c r="X1" s="5" t="inlineStr">
         <is>
           <t>Floor_Level</t>
         </is>
       </c>
-      <c r="Y1" s="4" t="inlineStr">
+      <c r="Y1" s="5" t="inlineStr">
         <is>
           <t>View</t>
         </is>
       </c>
-      <c r="Z1" s="4" t="inlineStr">
+      <c r="Z1" s="5" t="inlineStr">
         <is>
           <t>Furnishing</t>
         </is>
       </c>
-      <c r="AA1" s="4" t="inlineStr">
+      <c r="AA1" s="5" t="inlineStr">
         <is>
           <t>Parking</t>
         </is>
       </c>
-      <c r="AB1" s="4" t="inlineStr">
+      <c r="AB1" s="5" t="inlineStr">
         <is>
           <t>Facilities</t>
         </is>
       </c>
-      <c r="AC1" s="4" t="inlineStr">
+      <c r="AC1" s="5" t="inlineStr">
         <is>
           <t>Condition</t>
         </is>
       </c>
-      <c r="AD1" s="4" t="inlineStr">
+      <c r="AD1" s="5" t="inlineStr">
         <is>
           <t>Year_Built</t>
         </is>
       </c>
-      <c r="AE1" s="4" t="inlineStr">
+      <c r="AE1" s="5" t="inlineStr">
         <is>
           <t>Year_Renovated</t>
         </is>
       </c>
-      <c r="AF1" s="4" t="inlineStr">
+      <c r="AF1" s="5" t="inlineStr">
         <is>
           <t>Title_Deed</t>
         </is>
       </c>
-      <c r="AG1" s="4" t="inlineStr">
+      <c r="AG1" s="5" t="inlineStr">
         <is>
           <t>Developer</t>
         </is>
       </c>
-      <c r="AH1" s="4" t="inlineStr">
+      <c r="AH1" s="5" t="inlineStr">
         <is>
           <t>Photos_Link</t>
         </is>
       </c>
-      <c r="AI1" s="4" t="inlineStr">
+      <c r="AI1" s="5" t="inlineStr">
         <is>
           <t>Video_Link</t>
         </is>
       </c>
-      <c r="AJ1" s="4" t="inlineStr">
+      <c r="AJ1" s="5" t="inlineStr">
         <is>
           <t>Brochure_Link</t>
         </is>
       </c>
-      <c r="AK1" s="4" t="inlineStr">
+      <c r="AK1" s="5" t="inlineStr">
         <is>
           <t>Virtual_Tour</t>
         </is>
       </c>
-      <c r="AL1" s="4" t="inlineStr">
+      <c r="AL1" s="5" t="inlineStr">
         <is>
           <t>Listing_URL</t>
         </is>
       </c>
-      <c r="AM1" s="4" t="inlineStr">
+      <c r="AM1" s="5" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="AN1" s="4" t="inlineStr">
+      <c r="AN1" s="5" t="inlineStr">
         <is>
           <t>Source_Contact</t>
         </is>
       </c>
-      <c r="AO1" s="4" t="inlineStr">
+      <c r="AO1" s="5" t="inlineStr">
         <is>
           <t>Assigned_Agent</t>
         </is>
       </c>
-      <c r="AP1" s="4" t="inlineStr">
+      <c r="AP1" s="5" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="AQ1" s="4" t="inlineStr">
+      <c r="AQ1" s="5" t="inlineStr">
         <is>
           <t>Featured</t>
         </is>
       </c>
-      <c r="AR1" s="4" t="inlineStr">
+      <c r="AR1" s="5" t="inlineStr">
         <is>
           <t>Active_Marketing</t>
         </is>
       </c>
-      <c r="AS1" s="4" t="inlineStr">
+      <c r="AS1" s="5" t="inlineStr">
         <is>
           <t>Date_Added</t>
         </is>
       </c>
-      <c r="AT1" s="4" t="inlineStr">
+      <c r="AT1" s="5" t="inlineStr">
         <is>
           <t>Date_Updated</t>
         </is>
       </c>
-      <c r="AU1" s="4" t="inlineStr">
+      <c r="AU1" s="5" t="inlineStr">
         <is>
           <t>Date_Available</t>
         </is>
       </c>
-      <c r="AV1" s="4" t="inlineStr">
+      <c r="AV1" s="5" t="inlineStr">
         <is>
           <t>Views_Count</t>
         </is>
       </c>
-      <c r="AW1" s="4" t="inlineStr">
+      <c r="AW1" s="5" t="inlineStr">
         <is>
           <t>Viewings_Count</t>
         </is>
       </c>
-      <c r="AX1" s="4" t="inlineStr">
+      <c r="AX1" s="5" t="inlineStr">
         <is>
           <t>Notes_Internal</t>
         </is>
       </c>
-      <c r="AY1" s="4" t="inlineStr">
+      <c r="AY1" s="5" t="inlineStr">
         <is>
           <t>Tags</t>
         </is>
       </c>
-      <c r="AZ1" s="4" t="inlineStr">
+      <c r="AZ1" s="5" t="inlineStr">
         <is>
           <t>Language</t>
         </is>
       </c>
-      <c r="BA1" s="4" t="inlineStr">
+      <c r="BA1" s="5" t="inlineStr">
         <is>
           <t>WhatsApp_Message</t>
         </is>
       </c>
-      <c r="BB1" s="4" t="inlineStr">
+      <c r="BB1" s="5" t="inlineStr">
         <is>
           <t>QR_Code_URL</t>
         </is>
       </c>
-      <c r="BC1" s="4" t="inlineStr">
+      <c r="BC1" s="5" t="inlineStr">
         <is>
           <t>Print_Status</t>
         </is>
       </c>
-      <c r="BD1" s="4" t="inlineStr">
+      <c r="BD1" s="5" t="inlineStr">
         <is>
           <t>Print_Slot</t>
         </is>
       </c>
-      <c r="BE1" s="4" t="inlineStr">
+      <c r="BE1" s="5" t="inlineStr">
         <is>
           <t>FB_Posted_Date</t>
         </is>
       </c>
-      <c r="BF1" s="4" t="inlineStr">
+      <c r="BF1" s="5" t="inlineStr">
         <is>
           <t>FB_Post_Link</t>
         </is>
       </c>
-      <c r="BG1" s="4" t="inlineStr">
+      <c r="BG1" s="5" t="inlineStr">
         <is>
           <t>Website_Listed</t>
         </is>
       </c>
-      <c r="BH1" s="4" t="inlineStr">
+      <c r="BH1" s="5" t="inlineStr">
         <is>
           <t>Website_URL</t>
         </is>
       </c>
-      <c r="BI1" s="4" t="inlineStr">
+      <c r="BI1" s="5" t="inlineStr">
         <is>
           <t>Marketing_Priority</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="18">
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Available,Reserved,Sold,Rented,Pending,Off Market"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Project,Resale,Rental-LT,Rental-ST"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Condo,Villa,House,Townhouse,Land,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Pattaya City,Jomtien,Na Jomtien,Pratumnak,Wongamat,Bang Saray,Huay Yai,East Pattaya,Other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"THB,USD,EUR"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Freehold,Leasehold,Company"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No,N/A"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Unfurnished,Partly Furnished,Fully Furnished"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AC2:AC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"New,Excellent,Good,Fair,Needs Renovation"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AM2:AM1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Owner Direct,Agent,LINE Group,Facebook,Website,Walk-in,Referral"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AO2:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Somchai S.,Napat K.,John D.,Sarah M.,Unassigned"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AP2:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AQ2:AQ1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AR2:AR1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BC2:BC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BG2:BG1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="BI2:BI1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3195,7 +3912,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>PROPERTY MASTER LIST - README</t>
         </is>
@@ -3225,7 +3942,7 @@
       <c r="A6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>📋 TAB STRUCTURE:</t>
         </is>
@@ -3235,56 +3952,56 @@
       <c r="A8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="8" t="inlineStr">
         <is>
           <t>• 01_All_Properties - Main comprehensive list of all properties</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="inlineStr">
+      <c r="A10" s="8" t="inlineStr">
         <is>
           <t>• 02_Projects_New - New development projects only</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="8" t="inlineStr">
         <is>
           <t>• 03_Resale_Secondary - Secondary market properties</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="inlineStr">
+      <c r="A12" s="8" t="inlineStr">
         <is>
           <t>• 04_Rental_Long_Term - Long-term rental properties</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="inlineStr">
+      <c r="A13" s="8" t="inlineStr">
         <is>
           <t>• 05_Rental_Short_Term - Short-term/vacation rentals</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="inlineStr">
+      <c r="A14" s="8" t="inlineStr">
         <is>
           <t>• 06_Sold_Rented - Archive of completed transactions</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="inlineStr">
+      <c r="A15" s="8" t="inlineStr">
         <is>
           <t>• 07_Pending - Reserved or in-process properties</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="inlineStr">
+      <c r="A16" s="8" t="inlineStr">
         <is>
           <t>• README - This instructions tab</t>
         </is>
@@ -3294,7 +4011,7 @@
       <c r="A17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="inlineStr">
+      <c r="A18" s="7" t="inlineStr">
         <is>
           <t>🔧 GETTING STARTED:</t>
         </is>
@@ -3356,7 +4073,7 @@
       <c r="A27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="inlineStr">
+      <c r="A28" s="7" t="inlineStr">
         <is>
           <t>📝 REQUIRED FIELDS:</t>
         </is>
@@ -3366,63 +4083,63 @@
       <c r="A29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="7" t="inlineStr">
+      <c r="A30" s="8" t="inlineStr">
         <is>
           <t>• Property_ID (auto-generated)</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="7" t="inlineStr">
+      <c r="A31" s="8" t="inlineStr">
         <is>
           <t>• Status, Category, Type</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="7" t="inlineStr">
+      <c r="A32" s="8" t="inlineStr">
         <is>
           <t>• Project_Name</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="7" t="inlineStr">
+      <c r="A33" s="8" t="inlineStr">
         <is>
           <t>• Location_Area</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="7" t="inlineStr">
+      <c r="A34" s="8" t="inlineStr">
         <is>
           <t>• Bedrooms, Bathrooms, Size_SQM</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="7" t="inlineStr">
+      <c r="A35" s="8" t="inlineStr">
         <is>
           <t>• Photos_Link</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="7" t="inlineStr">
+      <c r="A36" s="8" t="inlineStr">
         <is>
           <t>• Assigned_Agent</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="7" t="inlineStr">
+      <c r="A37" s="8" t="inlineStr">
         <is>
           <t>• Active_Marketing</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="7" t="inlineStr">
+      <c r="A38" s="8" t="inlineStr">
         <is>
           <t>• Date_Added, Date_Updated</t>
         </is>
@@ -3432,7 +4149,7 @@
       <c r="A39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" s="6" t="inlineStr">
+      <c r="A40" s="7" t="inlineStr">
         <is>
           <t>🔍 TIPS:</t>
         </is>
@@ -3442,35 +4159,35 @@
       <c r="A41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" s="7" t="inlineStr">
+      <c r="A42" s="8" t="inlineStr">
         <is>
           <t>• Use Ctrl+F to search for properties</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="7" t="inlineStr">
+      <c r="A43" s="8" t="inlineStr">
         <is>
           <t>• Use filters on column headers for quick filtering</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="7" t="inlineStr">
+      <c r="A44" s="8" t="inlineStr">
         <is>
           <t>• Update Date_Updated whenever you modify a property</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="7" t="inlineStr">
+      <c r="A45" s="8" t="inlineStr">
         <is>
           <t>• Add internal notes in Notes_Internal column</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="7" t="inlineStr">
+      <c r="A46" s="8" t="inlineStr">
         <is>
           <t>• Review properties older than 90 days regularly</t>
         </is>
@@ -3480,7 +4197,7 @@
       <c r="A47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" s="6" t="inlineStr">
+      <c r="A48" s="7" t="inlineStr">
         <is>
           <t>📊 DATA QUALITY:</t>
         </is>
@@ -3490,35 +4207,35 @@
       <c r="A49" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" s="7" t="inlineStr">
+      <c r="A50" s="8" t="inlineStr">
         <is>
           <t>• Keep all property IDs unique</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="7" t="inlineStr">
+      <c r="A51" s="8" t="inlineStr">
         <is>
           <t>• Verify photo links are accessible</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="7" t="inlineStr">
+      <c r="A52" s="8" t="inlineStr">
         <is>
           <t>• Double-check prices for accuracy</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="7" t="inlineStr">
+      <c r="A53" s="8" t="inlineStr">
         <is>
           <t>• Use consistent date format (YYYY-MM-DD)</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="7" t="inlineStr">
+      <c r="A54" s="8" t="inlineStr">
         <is>
           <t>• Keep status up to date</t>
         </is>
@@ -3528,7 +4245,7 @@
       <c r="A55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" s="6" t="inlineStr">
+      <c r="A56" s="7" t="inlineStr">
         <is>
           <t>💡 For detailed documentation, see:</t>
         </is>

</xml_diff>